<commit_message>
integrated Danny's proofreading edits
</commit_message>
<xml_diff>
--- a/textbook_project_tracker.xlsx
+++ b/textbook_project_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Documents/Teaching/3505/NESC3505_textbook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Documents/Teaching/3505/NESC_3505_textbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A313EDE4-F0C7-2B46-957E-2B699840443B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE438A5-6599-FB43-A5BA-DED78E278030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="1680" windowWidth="16880" windowHeight="18240" xr2:uid="{FFE665D0-EDDA-8843-9D78-277E7A8C1336}"/>
+    <workbookView xWindow="1160" yWindow="3980" windowWidth="22600" windowHeight="18240" xr2:uid="{FFE665D0-EDDA-8843-9D78-277E7A8C1336}"/>
   </bookViews>
   <sheets>
     <sheet name="ch 1" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -75,9 +75,6 @@
     <t>reproducibility</t>
   </si>
   <si>
-    <t>go deeper</t>
-  </si>
-  <si>
     <t>sci_prog_lang</t>
   </si>
   <si>
@@ -145,13 +142,37 @@
   </si>
   <si>
     <t>mindset</t>
+  </si>
+  <si>
+    <t>proofread</t>
+  </si>
+  <si>
+    <t>data_sci_neurosci</t>
+  </si>
+  <si>
+    <t>data_sci_industry</t>
+  </si>
+  <si>
+    <t>Practical skills</t>
+  </si>
+  <si>
+    <t>course learning objectives</t>
+  </si>
+  <si>
+    <t>constructivism, connectionism</t>
+  </si>
+  <si>
+    <t>erros_debugging</t>
+  </si>
+  <si>
+    <t>teamwork</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,13 +184,6 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Gill Sans MT"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
       <name val="Gill Sans MT"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,17 +204,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -241,11 +250,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -265,19 +273,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,7 +505,154 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="37" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>43960</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="9">
+        <f>SUM(C2:C19)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476CA8DB-1F1A-3940-B4F7-DD9B618FB9E4}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,132 +686,6 @@
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
-        <v>43960</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="10">
-        <f>SUM(C2:C19)</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476CA8DB-1F1A-3940-B4F7-DD9B618FB9E4}">
-  <dimension ref="A1:F20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="37" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
         <v>43958</v>
       </c>
       <c r="B2" t="s">
@@ -675,17 +705,17 @@
       <c r="A3" s="6">
         <v>43958</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3">
-        <v>140</v>
+        <v>766</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -744,7 +774,7 @@
         <v>43958</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>414</v>
@@ -761,7 +791,7 @@
         <v>43958</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>612</v>
@@ -778,7 +808,7 @@
         <v>43958</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>736</v>
@@ -795,7 +825,7 @@
         <v>43958</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>61</v>
@@ -812,7 +842,7 @@
         <v>43958</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>259</v>
@@ -829,7 +859,7 @@
         <v>43958</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>657</v>
@@ -846,7 +876,7 @@
         <v>43958</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>916</v>
@@ -863,7 +893,7 @@
         <v>43958</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>583</v>
@@ -880,7 +910,7 @@
         <v>43958</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>240</v>
@@ -897,7 +927,7 @@
         <v>43958</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>491</v>
@@ -917,13 +947,13 @@
         <v>43959</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>1722</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -937,13 +967,13 @@
         <v>43958</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>324</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -957,28 +987,28 @@
         <v>43958</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>747</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <f>SUM(C2:C19)</f>
-        <v>9998</v>
+        <v>10624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added course learning objectives
</commit_message>
<xml_diff>
--- a/textbook_project_tracker.xlsx
+++ b/textbook_project_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Documents/Teaching/3505/NESC_3505_textbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE438A5-6599-FB43-A5BA-DED78E278030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C844BA-CEB9-6045-BB72-5C3A03FE4204}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="3980" windowWidth="22600" windowHeight="18240" xr2:uid="{FFE665D0-EDDA-8843-9D78-277E7A8C1336}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -147,18 +147,9 @@
     <t>proofread</t>
   </si>
   <si>
-    <t>data_sci_neurosci</t>
-  </si>
-  <si>
-    <t>data_sci_industry</t>
-  </si>
-  <si>
     <t>Practical skills</t>
   </si>
   <si>
-    <t>course learning objectives</t>
-  </si>
-  <si>
     <t>constructivism, connectionism</t>
   </si>
   <si>
@@ -166,6 +157,21 @@
   </si>
   <si>
     <t>teamwork</t>
+  </si>
+  <si>
+    <t>why</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>learning objectives (of course)</t>
+  </si>
+  <si>
+    <t>philosophy</t>
   </si>
 </sst>
 </file>
@@ -502,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A63BF6-29C6-274B-A30D-8186D7EB5130}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,25 +548,37 @@
         <v>43960</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>363</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -568,63 +586,63 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
-      <c r="B10" t="s">
-        <v>32</v>
+      <c r="B10" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
@@ -632,12 +650,12 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="9" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="9">
-        <f>SUM(C2:C19)</f>
+      <c r="C21" s="9">
+        <f>SUM(C3:C20)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished first draft of chapter 1
</commit_message>
<xml_diff>
--- a/textbook_project_tracker.xlsx
+++ b/textbook_project_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Documents/Teaching/3505/NESC_3505_textbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1FE685-3831-6F49-8A43-B39BFD1503A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53817110-D169-3F46-98B0-7012180231DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="6980" windowWidth="22600" windowHeight="18240" xr2:uid="{FFE665D0-EDDA-8843-9D78-277E7A8C1336}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="50">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -129,9 +129,6 @@
     <t>core_principles</t>
   </si>
   <si>
-    <t>values_goals</t>
-  </si>
-  <si>
     <t>mindset</t>
   </si>
   <si>
@@ -178,6 +175,15 @@
   </si>
   <si>
     <t>y (but look to add citations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open science </t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>oer</t>
   </si>
 </sst>
 </file>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A63BF6-29C6-274B-A30D-8186D7EB5130}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,13 +560,13 @@
         <v>43960</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2">
         <v>489</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -572,7 +578,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>294</v>
@@ -587,7 +593,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>664</v>
@@ -602,7 +608,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>384</v>
@@ -611,13 +617,13 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>467</v>
@@ -632,7 +638,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>426</v>
@@ -646,17 +652,20 @@
       <c r="B8" t="s">
         <v>30</v>
       </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10">
         <v>872</v>
@@ -671,55 +680,109 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>854</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="C13">
+        <v>3552</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>49</v>
+      </c>
+      <c r="C14">
+        <v>1449</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
+      <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="9" t="s">
+      <c r="A21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="9">
-        <f>SUM(C3:C20)</f>
-        <v>3107</v>
+      <c r="C24" s="9">
+        <f>SUM(C3:C23)</f>
+        <v>9116</v>
       </c>
     </row>
   </sheetData>
@@ -796,7 +859,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
jupyter book compile files
</commit_message>
<xml_diff>
--- a/textbook_project_tracker.xlsx
+++ b/textbook_project_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Documents/Teaching/3505/NESC_3505_textbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DEF870-80D8-F746-B9E1-2D39FF75809A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0A3E76-0A5C-B247-AC5B-9935B4930138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="6980" windowWidth="22600" windowHeight="18240" xr2:uid="{FFE665D0-EDDA-8843-9D78-277E7A8C1336}"/>
+    <workbookView xWindow="960" yWindow="7480" windowWidth="15100" windowHeight="18240" xr2:uid="{FFE665D0-EDDA-8843-9D78-277E7A8C1336}"/>
   </bookViews>
   <sheets>
     <sheet name="ch 1" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="48">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -126,9 +126,6 @@
     <t>why_python</t>
   </si>
   <si>
-    <t>core_principles</t>
-  </si>
-  <si>
     <t>proofread</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>oer</t>
+  </si>
+  <si>
+    <t>authenticity</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,13 +563,13 @@
         <v>43960</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>489</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -581,7 +581,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <v>294</v>
@@ -595,8 +595,8 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
-      <c r="B4" t="s">
-        <v>36</v>
+      <c r="B4" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C4">
         <v>664</v>
@@ -611,7 +611,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>384</v>
@@ -620,16 +620,16 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
-      <c r="B6" t="s">
-        <v>38</v>
+      <c r="B6" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="C6">
-        <v>467</v>
+        <v>872</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -641,10 +641,10 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7">
-        <v>426</v>
+        <v>467</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -655,11 +655,11 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
-      <c r="B8" s="10" t="s">
-        <v>30</v>
+      <c r="B8" t="s">
+        <v>38</v>
       </c>
       <c r="C8">
-        <v>30</v>
+        <v>426</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -671,10 +671,10 @@
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="11" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C9">
-        <v>872</v>
+        <v>413</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -685,8 +685,8 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
-      <c r="B10" t="s">
-        <v>41</v>
+      <c r="B10" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C10">
         <v>124</v>
@@ -701,7 +701,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <v>854</v>
@@ -716,7 +716,7 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>3552</v>
@@ -731,7 +731,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>1449</v>
@@ -746,16 +746,22 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <v>296</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>687</v>
@@ -770,7 +776,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>381</v>
@@ -788,7 +794,7 @@
       </c>
       <c r="C17" s="9">
         <f>SUM(C3:C16)</f>
-        <v>10480</v>
+        <v>10863</v>
       </c>
     </row>
   </sheetData>
@@ -865,7 +871,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>